<commit_message>
Need to insert into template differently for styling probably
</commit_message>
<xml_diff>
--- a/data/Templates/UnionSpecial.xlsx
+++ b/data/Templates/UnionSpecial.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/david/xtractor/data/Templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{808E18C3-0B75-B649-B78D-051AEB7DE00C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF7956C2-12BA-5F41-B117-414C5D72A6AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -326,7 +326,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -462,11 +462,59 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -540,7 +588,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -548,8 +595,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -565,11 +614,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -592,14 +636,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -610,9 +646,21 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1567,8 +1615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="193" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" zoomScale="193" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10:H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
@@ -1585,158 +1633,158 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
-      <c r="A1" s="48"/>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
+      <c r="A1" s="47"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
     </row>
     <row r="2" spans="1:17">
-      <c r="A2" s="49"/>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
+      <c r="A2" s="48"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
     </row>
     <row r="3" spans="1:17">
-      <c r="A3" s="49"/>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="49"/>
-      <c r="G3" s="49"/>
-      <c r="H3" s="49"/>
+      <c r="A3" s="48"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="48"/>
     </row>
     <row r="4" spans="1:17" ht="12.75" customHeight="1">
-      <c r="A4" s="57" t="s">
+      <c r="A4" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="49"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
-      <c r="F4" s="49"/>
-      <c r="G4" s="49"/>
-      <c r="H4" s="49"/>
+      <c r="B4" s="48"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="48"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="48"/>
+      <c r="H4" s="48"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
     <row r="5" spans="1:17" ht="12.75" customHeight="1">
-      <c r="A5" s="50" t="s">
+      <c r="A5" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="49"/>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
+      <c r="B5" s="48"/>
+      <c r="C5" s="48"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="48"/>
       <c r="I5" s="1"/>
-      <c r="J5" s="41"/>
+      <c r="J5" s="40"/>
     </row>
     <row r="6" spans="1:17" ht="12.75" customHeight="1">
-      <c r="A6" s="50" t="s">
+      <c r="A6" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="49"/>
-      <c r="C6" s="49"/>
-      <c r="D6" s="49"/>
-      <c r="E6" s="49"/>
-      <c r="F6" s="49"/>
-      <c r="G6" s="49"/>
-      <c r="H6" s="49"/>
+      <c r="B6" s="48"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="48"/>
+      <c r="F6" s="48"/>
+      <c r="G6" s="48"/>
+      <c r="H6" s="48"/>
       <c r="I6" s="1"/>
-      <c r="J6" s="41"/>
+      <c r="J6" s="40"/>
     </row>
     <row r="7" spans="1:17" ht="12.75" customHeight="1">
-      <c r="A7" s="58" t="s">
+      <c r="A7" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="49"/>
-      <c r="C7" s="49"/>
-      <c r="D7" s="49"/>
-      <c r="E7" s="49"/>
-      <c r="F7" s="49"/>
-      <c r="G7" s="49"/>
-      <c r="H7" s="49"/>
+      <c r="B7" s="48"/>
+      <c r="C7" s="48"/>
+      <c r="D7" s="48"/>
+      <c r="E7" s="48"/>
+      <c r="F7" s="48"/>
+      <c r="G7" s="48"/>
+      <c r="H7" s="48"/>
       <c r="I7" s="1"/>
-      <c r="J7" s="41"/>
+      <c r="J7" s="40"/>
     </row>
     <row r="8" spans="1:17" ht="12.75" customHeight="1">
-      <c r="A8" s="55" t="s">
+      <c r="A8" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="49"/>
-      <c r="C8" s="49"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="49"/>
-      <c r="F8" s="49"/>
-      <c r="G8" s="49"/>
-      <c r="H8" s="49"/>
-      <c r="I8" s="41"/>
-      <c r="J8" s="41"/>
+      <c r="B8" s="48"/>
+      <c r="C8" s="48"/>
+      <c r="D8" s="48"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="48"/>
+      <c r="G8" s="48"/>
+      <c r="H8" s="48"/>
+      <c r="I8" s="40"/>
+      <c r="J8" s="40"/>
     </row>
     <row r="9" spans="1:17" ht="12.75" customHeight="1">
-      <c r="A9" s="42"/>
-      <c r="B9" s="42"/>
-      <c r="C9" s="42"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="42"/>
-      <c r="F9" s="42"/>
-      <c r="G9" s="42"/>
-      <c r="H9" s="42"/>
-      <c r="I9" s="41"/>
-      <c r="J9" s="41"/>
+      <c r="A9" s="41"/>
+      <c r="B9" s="41"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="40"/>
+      <c r="J9" s="40"/>
     </row>
     <row r="10" spans="1:17" s="16" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A10" s="51" t="s">
+      <c r="A10" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="46"/>
-      <c r="C10" s="46"/>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46"/>
+      <c r="B10" s="45"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="45"/>
       <c r="F10" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="G10" s="45">
+      <c r="G10" s="44">
         <v>43801</v>
       </c>
-      <c r="H10" s="46"/>
+      <c r="H10" s="45"/>
     </row>
     <row r="11" spans="1:17" s="16" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A11" s="51" t="s">
+      <c r="A11" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="46"/>
-      <c r="C11" s="46"/>
-      <c r="D11" s="46"/>
-      <c r="E11" s="46"/>
+      <c r="B11" s="45"/>
+      <c r="C11" s="45"/>
+      <c r="D11" s="45"/>
+      <c r="E11" s="45"/>
       <c r="F11" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="G11" s="45">
+      <c r="G11" s="44">
         <v>43801</v>
       </c>
-      <c r="H11" s="46"/>
+      <c r="H11" s="45"/>
     </row>
     <row r="12" spans="1:17" s="16" customFormat="1" ht="12.75" customHeight="1">
       <c r="A12" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="56">
+      <c r="F12" s="52">
         <v>12148</v>
       </c>
-      <c r="G12" s="46"/>
-      <c r="H12" s="46"/>
+      <c r="G12" s="45"/>
+      <c r="H12" s="45"/>
     </row>
     <row r="13" spans="1:17" s="16" customFormat="1" ht="12.75" customHeight="1">
       <c r="A13" s="16" t="s">
@@ -1749,16 +1797,16 @@
       <c r="J14" s="20"/>
     </row>
     <row r="15" spans="1:17" s="16" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A15" s="59" t="s">
+      <c r="A15" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="46"/>
-      <c r="C15" s="46"/>
-      <c r="D15" s="46"/>
-      <c r="E15" s="46"/>
-      <c r="F15" s="46"/>
-      <c r="G15" s="46"/>
-      <c r="H15" s="46"/>
+      <c r="B15" s="45"/>
+      <c r="C15" s="45"/>
+      <c r="D15" s="45"/>
+      <c r="E15" s="45"/>
+      <c r="F15" s="45"/>
+      <c r="G15" s="45"/>
+      <c r="H15" s="45"/>
       <c r="I15" s="36"/>
       <c r="J15" s="20"/>
     </row>
@@ -1781,26 +1829,26 @@
       <c r="F16" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="G16" s="52" t="s">
+      <c r="G16" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="H16" s="44"/>
+      <c r="H16" s="74"/>
       <c r="I16" s="38" t="s">
         <v>19</v>
       </c>
       <c r="J16" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="K16" s="71" t="s">
+      <c r="K16" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="L16" s="71" t="s">
+      <c r="L16" s="42" t="s">
         <v>48</v>
       </c>
-      <c r="M16" s="71" t="s">
+      <c r="M16" s="42" t="s">
         <v>49</v>
       </c>
-      <c r="N16" s="71" t="s">
+      <c r="N16" s="42" t="s">
         <v>50</v>
       </c>
       <c r="P16" s="25"/>
@@ -1819,18 +1867,18 @@
       <c r="D17" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="E17" s="40" t="s">
+      <c r="E17" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="F17" s="39">
+      <c r="F17" s="72">
         <f>J17</f>
         <v>623.15599999999995</v>
       </c>
-      <c r="G17" s="43">
+      <c r="G17" s="75"/>
+      <c r="H17" s="76">
         <f>F17*B17</f>
         <v>0</v>
       </c>
-      <c r="H17" s="44"/>
       <c r="I17" s="35">
         <v>289.83999999999997</v>
       </c>
@@ -1848,10 +1896,10 @@
       <c r="B18" s="30"/>
       <c r="C18" s="31"/>
       <c r="D18" s="26"/>
-      <c r="E18" s="40"/>
-      <c r="F18" s="39"/>
-      <c r="G18" s="43"/>
-      <c r="H18" s="44"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="72"/>
+      <c r="G18" s="77"/>
+      <c r="H18" s="43"/>
       <c r="I18" s="35"/>
       <c r="J18" s="35"/>
       <c r="K18" s="35"/>
@@ -1859,12 +1907,12 @@
     </row>
     <row r="19" spans="1:17" s="16" customFormat="1" ht="12.75" customHeight="1" thickBot="1">
       <c r="A19" s="17"/>
-      <c r="B19" s="41"/>
-      <c r="C19" s="41"/>
+      <c r="B19" s="40"/>
+      <c r="C19" s="40"/>
       <c r="D19" s="18"/>
       <c r="F19" s="19"/>
-      <c r="G19" s="47"/>
-      <c r="H19" s="46"/>
+      <c r="G19" s="63"/>
+      <c r="H19" s="64"/>
       <c r="I19" s="35"/>
       <c r="J19" s="35"/>
       <c r="K19" s="35"/>
@@ -1872,18 +1920,18 @@
     </row>
     <row r="20" spans="1:17" s="16" customFormat="1" ht="12.75" customHeight="1">
       <c r="A20" s="17"/>
-      <c r="B20" s="41"/>
-      <c r="C20" s="41"/>
+      <c r="B20" s="40"/>
+      <c r="C20" s="40"/>
       <c r="D20" s="18"/>
-      <c r="E20" s="60" t="s">
+      <c r="E20" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="61"/>
-      <c r="G20" s="65">
-        <f>SUM(G17:G19)</f>
+      <c r="F20" s="57"/>
+      <c r="G20" s="69"/>
+      <c r="H20" s="65">
+        <f>SUM(H17:H19)</f>
         <v>0</v>
       </c>
-      <c r="H20" s="66"/>
       <c r="I20" s="35"/>
       <c r="J20" s="35"/>
       <c r="K20" s="35"/>
@@ -1894,15 +1942,15 @@
       <c r="B21" s="17"/>
       <c r="C21" s="17"/>
       <c r="D21" s="21"/>
-      <c r="E21" s="70" t="s">
+      <c r="E21" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="F21" s="46"/>
-      <c r="G21" s="63">
-        <f>G20*25/100</f>
+      <c r="F21" s="70"/>
+      <c r="G21" s="68"/>
+      <c r="H21" s="66">
+        <f>H20*25/100</f>
         <v>0</v>
       </c>
-      <c r="H21" s="64"/>
       <c r="I21" s="7"/>
       <c r="J21" s="35"/>
       <c r="K21" s="35"/>
@@ -1913,15 +1961,15 @@
       <c r="B22" s="17"/>
       <c r="C22" s="17"/>
       <c r="D22" s="21"/>
-      <c r="E22" s="68" t="s">
+      <c r="E22" s="60" t="s">
         <v>23</v>
       </c>
-      <c r="F22" s="69"/>
-      <c r="G22" s="53">
-        <f>G20-G21</f>
+      <c r="F22" s="61"/>
+      <c r="G22" s="71"/>
+      <c r="H22" s="67">
+        <f>H20-H21</f>
         <v>0</v>
       </c>
-      <c r="H22" s="54"/>
       <c r="I22" s="7"/>
       <c r="J22" s="35"/>
       <c r="K22" s="35"/>
@@ -1933,8 +1981,8 @@
       <c r="C23" s="17"/>
       <c r="D23" s="21"/>
       <c r="F23" s="19"/>
-      <c r="G23" s="47"/>
-      <c r="H23" s="46"/>
+      <c r="G23" s="46"/>
+      <c r="H23" s="45"/>
       <c r="I23" s="22"/>
       <c r="J23" s="35"/>
       <c r="K23" s="35"/>
@@ -2096,12 +2144,12 @@
       <c r="B39" s="13"/>
       <c r="C39" s="13"/>
       <c r="D39" s="13"/>
-      <c r="E39" s="67" t="s">
+      <c r="E39" s="59" t="s">
         <v>41</v>
       </c>
-      <c r="F39" s="49"/>
-      <c r="G39" s="49"/>
-      <c r="H39" s="49"/>
+      <c r="F39" s="48"/>
+      <c r="G39" s="48"/>
+      <c r="H39" s="48"/>
     </row>
     <row r="40" spans="1:8" ht="14" customHeight="1">
       <c r="A40" s="13"/>
@@ -2207,9 +2255,9 @@
       <c r="G55" s="16"/>
     </row>
     <row r="56" spans="1:8">
-      <c r="F56" s="62"/>
-      <c r="G56" s="49"/>
-      <c r="H56" s="49"/>
+      <c r="F56" s="58"/>
+      <c r="G56" s="48"/>
+      <c r="H56" s="48"/>
     </row>
     <row r="57" spans="1:8">
       <c r="A57" s="16"/>
@@ -2224,32 +2272,25 @@
       <c r="H60" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="25">
-    <mergeCell ref="A15:H15"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="E20:F20"/>
+  <mergeCells count="18">
     <mergeCell ref="F56:H56"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="G20:H20"/>
     <mergeCell ref="E39:H39"/>
     <mergeCell ref="E22:F22"/>
     <mergeCell ref="E21:F21"/>
-    <mergeCell ref="G17:H17"/>
     <mergeCell ref="G11:H11"/>
     <mergeCell ref="G23:H23"/>
     <mergeCell ref="A1:H3"/>
     <mergeCell ref="A5:H5"/>
     <mergeCell ref="A10:E10"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="G22:H22"/>
     <mergeCell ref="A11:E11"/>
     <mergeCell ref="A8:H8"/>
     <mergeCell ref="F12:H12"/>
     <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G18:H18"/>
     <mergeCell ref="A4:H4"/>
     <mergeCell ref="A6:H6"/>
     <mergeCell ref="A7:H7"/>
+    <mergeCell ref="A15:H15"/>
+    <mergeCell ref="E20:F20"/>
   </mergeCells>
   <pageMargins left="3.937007874015748E-2" right="0.43307086614173229" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125978" footer="0.31496062992125978"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Making the excel output more robust ..
</commit_message>
<xml_diff>
--- a/data/Templates/UnionSpecial.xlsx
+++ b/data/Templates/UnionSpecial.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/david/xtractor/data/Templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF7956C2-12BA-5F41-B117-414C5D72A6AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3BC3E2C-E7A0-2348-AF36-2AEF674C1BDE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -599,61 +599,10 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -661,6 +610,53 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -738,7 +734,7 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>101600</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>38101</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -789,7 +785,7 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>165100</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>38101</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -840,7 +836,7 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>609600</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>38101</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -891,7 +887,7 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>101600</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>38101</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -942,7 +938,7 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>723900</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>38101</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -993,7 +989,7 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>1206500</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>38101</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1044,7 +1040,7 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>1968500</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>38101</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1095,7 +1091,7 @@
       <xdr:col>5</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>38101</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1146,7 +1142,7 @@
       <xdr:col>5</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>38101</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1197,7 +1193,7 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>165100</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>38101</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1248,7 +1244,7 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>571500</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>38101</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1615,8 +1611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="193" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10:H10"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="193" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
@@ -1633,102 +1629,102 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
-      <c r="A1" s="47"/>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
+      <c r="A1" s="72"/>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
     </row>
     <row r="2" spans="1:17">
-      <c r="A2" s="48"/>
-      <c r="B2" s="48"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
+      <c r="A2" s="67"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
     </row>
     <row r="3" spans="1:17">
-      <c r="A3" s="48"/>
-      <c r="B3" s="48"/>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="48"/>
+      <c r="A3" s="67"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="67"/>
     </row>
     <row r="4" spans="1:17" ht="12.75" customHeight="1">
-      <c r="A4" s="53" t="s">
+      <c r="A4" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="48"/>
-      <c r="C4" s="48"/>
-      <c r="D4" s="48"/>
-      <c r="E4" s="48"/>
-      <c r="F4" s="48"/>
-      <c r="G4" s="48"/>
-      <c r="H4" s="48"/>
+      <c r="B4" s="67"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="67"/>
+      <c r="G4" s="67"/>
+      <c r="H4" s="67"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
     <row r="5" spans="1:17" ht="12.75" customHeight="1">
-      <c r="A5" s="49" t="s">
+      <c r="A5" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="48"/>
-      <c r="C5" s="48"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="48"/>
-      <c r="G5" s="48"/>
-      <c r="H5" s="48"/>
+      <c r="B5" s="67"/>
+      <c r="C5" s="67"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="67"/>
+      <c r="H5" s="67"/>
       <c r="I5" s="1"/>
       <c r="J5" s="40"/>
     </row>
     <row r="6" spans="1:17" ht="12.75" customHeight="1">
-      <c r="A6" s="49" t="s">
+      <c r="A6" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="48"/>
-      <c r="C6" s="48"/>
-      <c r="D6" s="48"/>
-      <c r="E6" s="48"/>
-      <c r="F6" s="48"/>
-      <c r="G6" s="48"/>
-      <c r="H6" s="48"/>
+      <c r="B6" s="67"/>
+      <c r="C6" s="67"/>
+      <c r="D6" s="67"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="67"/>
+      <c r="G6" s="67"/>
+      <c r="H6" s="67"/>
       <c r="I6" s="1"/>
       <c r="J6" s="40"/>
     </row>
     <row r="7" spans="1:17" ht="12.75" customHeight="1">
-      <c r="A7" s="54" t="s">
+      <c r="A7" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="48"/>
-      <c r="C7" s="48"/>
-      <c r="D7" s="48"/>
-      <c r="E7" s="48"/>
-      <c r="F7" s="48"/>
-      <c r="G7" s="48"/>
-      <c r="H7" s="48"/>
+      <c r="B7" s="67"/>
+      <c r="C7" s="67"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="67"/>
+      <c r="H7" s="67"/>
       <c r="I7" s="1"/>
       <c r="J7" s="40"/>
     </row>
     <row r="8" spans="1:17" ht="12.75" customHeight="1">
-      <c r="A8" s="51" t="s">
+      <c r="A8" s="75" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="48"/>
-      <c r="C8" s="48"/>
-      <c r="D8" s="48"/>
-      <c r="E8" s="48"/>
-      <c r="F8" s="48"/>
-      <c r="G8" s="48"/>
-      <c r="H8" s="48"/>
+      <c r="B8" s="67"/>
+      <c r="C8" s="67"/>
+      <c r="D8" s="67"/>
+      <c r="E8" s="67"/>
+      <c r="F8" s="67"/>
+      <c r="G8" s="67"/>
+      <c r="H8" s="67"/>
       <c r="I8" s="40"/>
       <c r="J8" s="40"/>
     </row>
@@ -1745,46 +1741,46 @@
       <c r="J9" s="40"/>
     </row>
     <row r="10" spans="1:17" s="16" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A10" s="50" t="s">
+      <c r="A10" s="74" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="45"/>
-      <c r="C10" s="45"/>
-      <c r="D10" s="45"/>
-      <c r="E10" s="45"/>
+      <c r="B10" s="69"/>
+      <c r="C10" s="69"/>
+      <c r="D10" s="69"/>
+      <c r="E10" s="69"/>
       <c r="F10" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="G10" s="44">
+      <c r="G10" s="68">
         <v>43801</v>
       </c>
-      <c r="H10" s="45"/>
+      <c r="H10" s="69"/>
     </row>
     <row r="11" spans="1:17" s="16" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A11" s="50" t="s">
+      <c r="A11" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="45"/>
-      <c r="C11" s="45"/>
-      <c r="D11" s="45"/>
-      <c r="E11" s="45"/>
+      <c r="B11" s="69"/>
+      <c r="C11" s="69"/>
+      <c r="D11" s="69"/>
+      <c r="E11" s="69"/>
       <c r="F11" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="G11" s="44">
+      <c r="G11" s="68">
         <v>43801</v>
       </c>
-      <c r="H11" s="45"/>
+      <c r="H11" s="69"/>
     </row>
     <row r="12" spans="1:17" s="16" customFormat="1" ht="12.75" customHeight="1">
       <c r="A12" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="52">
+      <c r="F12" s="70">
         <v>12148</v>
       </c>
-      <c r="G12" s="45"/>
-      <c r="H12" s="45"/>
+      <c r="G12" s="69"/>
+      <c r="H12" s="69"/>
     </row>
     <row r="13" spans="1:17" s="16" customFormat="1" ht="12.75" customHeight="1">
       <c r="A13" s="16" t="s">
@@ -1797,16 +1793,16 @@
       <c r="J14" s="20"/>
     </row>
     <row r="15" spans="1:17" s="16" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A15" s="55" t="s">
+      <c r="A15" s="71" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="45"/>
-      <c r="C15" s="45"/>
-      <c r="D15" s="45"/>
-      <c r="E15" s="45"/>
-      <c r="F15" s="45"/>
-      <c r="G15" s="45"/>
-      <c r="H15" s="45"/>
+      <c r="B15" s="69"/>
+      <c r="C15" s="69"/>
+      <c r="D15" s="69"/>
+      <c r="E15" s="69"/>
+      <c r="F15" s="69"/>
+      <c r="G15" s="69"/>
+      <c r="H15" s="69"/>
       <c r="I15" s="36"/>
       <c r="J15" s="20"/>
     </row>
@@ -1829,10 +1825,10 @@
       <c r="F16" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="G16" s="73" t="s">
+      <c r="G16" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="H16" s="74"/>
+      <c r="H16" s="51"/>
       <c r="I16" s="38" t="s">
         <v>19</v>
       </c>
@@ -1870,12 +1866,12 @@
       <c r="E17" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="F17" s="72">
+      <c r="F17" s="49">
         <f>J17</f>
         <v>623.15599999999995</v>
       </c>
-      <c r="G17" s="75"/>
-      <c r="H17" s="76">
+      <c r="G17" s="52"/>
+      <c r="H17" s="53">
         <f>F17*B17</f>
         <v>0</v>
       </c>
@@ -1897,22 +1893,22 @@
       <c r="C18" s="31"/>
       <c r="D18" s="26"/>
       <c r="E18" s="39"/>
-      <c r="F18" s="72"/>
-      <c r="G18" s="77"/>
+      <c r="F18" s="49"/>
+      <c r="G18" s="54"/>
       <c r="H18" s="43"/>
       <c r="I18" s="35"/>
       <c r="J18" s="35"/>
       <c r="K18" s="35"/>
       <c r="L18" s="20"/>
     </row>
-    <row r="19" spans="1:17" s="16" customFormat="1" ht="12.75" customHeight="1" thickBot="1">
+    <row r="19" spans="1:17" s="16" customFormat="1" ht="14" customHeight="1" thickBot="1">
       <c r="A19" s="17"/>
       <c r="B19" s="40"/>
       <c r="C19" s="40"/>
       <c r="D19" s="18"/>
       <c r="F19" s="19"/>
-      <c r="G19" s="63"/>
-      <c r="H19" s="64"/>
+      <c r="G19" s="44"/>
+      <c r="H19" s="45"/>
       <c r="I19" s="35"/>
       <c r="J19" s="35"/>
       <c r="K19" s="35"/>
@@ -1923,12 +1919,12 @@
       <c r="B20" s="40"/>
       <c r="C20" s="40"/>
       <c r="D20" s="18"/>
-      <c r="E20" s="56" t="s">
+      <c r="E20" s="59" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="57"/>
-      <c r="G20" s="69"/>
-      <c r="H20" s="65">
+      <c r="F20" s="60"/>
+      <c r="G20" s="47"/>
+      <c r="H20" s="63">
         <f>SUM(H17:H19)</f>
         <v>0</v>
       </c>
@@ -1942,12 +1938,12 @@
       <c r="B21" s="17"/>
       <c r="C21" s="17"/>
       <c r="D21" s="21"/>
-      <c r="E21" s="62" t="s">
+      <c r="E21" s="57" t="s">
         <v>22</v>
       </c>
-      <c r="F21" s="70"/>
-      <c r="G21" s="68"/>
-      <c r="H21" s="66">
+      <c r="F21" s="58"/>
+      <c r="G21" s="46"/>
+      <c r="H21" s="64">
         <f>H20*25/100</f>
         <v>0</v>
       </c>
@@ -1961,12 +1957,12 @@
       <c r="B22" s="17"/>
       <c r="C22" s="17"/>
       <c r="D22" s="21"/>
-      <c r="E22" s="60" t="s">
+      <c r="E22" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="F22" s="61"/>
-      <c r="G22" s="71"/>
-      <c r="H22" s="67">
+      <c r="F22" s="56"/>
+      <c r="G22" s="48"/>
+      <c r="H22" s="65">
         <f>H20-H21</f>
         <v>0</v>
       </c>
@@ -1981,7 +1977,7 @@
       <c r="C23" s="17"/>
       <c r="D23" s="21"/>
       <c r="F23" s="19"/>
-      <c r="G23" s="46"/>
+      <c r="G23" s="44"/>
       <c r="H23" s="45"/>
       <c r="I23" s="22"/>
       <c r="J23" s="35"/>
@@ -2144,12 +2140,12 @@
       <c r="B39" s="13"/>
       <c r="C39" s="13"/>
       <c r="D39" s="13"/>
-      <c r="E39" s="59" t="s">
+      <c r="E39" s="61" t="s">
         <v>41</v>
       </c>
-      <c r="F39" s="48"/>
-      <c r="G39" s="48"/>
-      <c r="H39" s="48"/>
+      <c r="F39" s="62"/>
+      <c r="G39" s="62"/>
+      <c r="H39" s="62"/>
     </row>
     <row r="40" spans="1:8" ht="14" customHeight="1">
       <c r="A40" s="13"/>
@@ -2255,9 +2251,9 @@
       <c r="G55" s="16"/>
     </row>
     <row r="56" spans="1:8">
-      <c r="F56" s="58"/>
-      <c r="G56" s="48"/>
-      <c r="H56" s="48"/>
+      <c r="F56" s="66"/>
+      <c r="G56" s="67"/>
+      <c r="H56" s="67"/>
     </row>
     <row r="57" spans="1:8">
       <c r="A57" s="16"/>
@@ -2272,25 +2268,20 @@
       <c r="H60" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="13">
     <mergeCell ref="F56:H56"/>
-    <mergeCell ref="E39:H39"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E21:F21"/>
     <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="A15:H15"/>
     <mergeCell ref="A1:H3"/>
     <mergeCell ref="A5:H5"/>
     <mergeCell ref="A10:E10"/>
     <mergeCell ref="A11:E11"/>
     <mergeCell ref="A8:H8"/>
-    <mergeCell ref="F12:H12"/>
     <mergeCell ref="G10:H10"/>
     <mergeCell ref="A4:H4"/>
     <mergeCell ref="A6:H6"/>
     <mergeCell ref="A7:H7"/>
-    <mergeCell ref="A15:H15"/>
-    <mergeCell ref="E20:F20"/>
   </mergeCells>
   <pageMargins left="3.937007874015748E-2" right="0.43307086614173229" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125978" footer="0.31496062992125978"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Single attachments seem to work. Now testing multi attachments again
</commit_message>
<xml_diff>
--- a/data/Templates/UnionSpecial.xlsx
+++ b/data/Templates/UnionSpecial.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/david/xtractor/data/Templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3BC3E2C-E7A0-2348-AF36-2AEF674C1BDE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44DE0D06-04B2-6849-9A5B-6661FB06C2BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1611,8 +1611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="193" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="193" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
@@ -2169,7 +2169,7 @@
       <c r="G41" s="23"/>
       <c r="H41" s="34"/>
     </row>
-    <row r="42" spans="1:8" ht="7.5" customHeight="1">
+    <row r="42" spans="1:8" ht="14" customHeight="1">
       <c r="A42" s="13"/>
       <c r="B42" s="13"/>
       <c r="C42" s="13"/>

</xml_diff>

<commit_message>
Struggling with byteencodings #1
</commit_message>
<xml_diff>
--- a/data/Templates/UnionSpecial.xlsx
+++ b/data/Templates/UnionSpecial.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/david/xtractor/data/Templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44DE0D06-04B2-6849-9A5B-6661FB06C2BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92B8D3FD-FFCF-3E4C-BB33-EB6DF07CCA1A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -627,17 +627,15 @@
     <xf numFmtId="164" fontId="7" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1611,8 +1609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="193" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView tabSelected="1" zoomScale="193" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
@@ -1623,52 +1621,52 @@
     <col min="4" max="4" width="13.6640625" style="10" customWidth="1"/>
     <col min="5" max="5" width="31.5" style="10" customWidth="1"/>
     <col min="6" max="6" width="13.6640625" style="10" customWidth="1"/>
-    <col min="8" max="8" width="7.5" style="10" customWidth="1"/>
+    <col min="8" max="8" width="9" style="10" customWidth="1"/>
     <col min="9" max="10" width="11.6640625" style="10" customWidth="1"/>
     <col min="11" max="11" width="10.6640625" style="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
       <c r="A1" s="72"/>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="67"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
     </row>
     <row r="2" spans="1:17">
-      <c r="A2" s="67"/>
-      <c r="B2" s="67"/>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
+      <c r="A2" s="68"/>
+      <c r="B2" s="68"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="68"/>
+      <c r="H2" s="68"/>
     </row>
     <row r="3" spans="1:17">
-      <c r="A3" s="67"/>
-      <c r="B3" s="67"/>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
-      <c r="F3" s="67"/>
-      <c r="G3" s="67"/>
-      <c r="H3" s="67"/>
+      <c r="A3" s="68"/>
+      <c r="B3" s="68"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="68"/>
+      <c r="G3" s="68"/>
+      <c r="H3" s="68"/>
     </row>
     <row r="4" spans="1:17" ht="12.75" customHeight="1">
       <c r="A4" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="67"/>
-      <c r="C4" s="67"/>
-      <c r="D4" s="67"/>
-      <c r="E4" s="67"/>
-      <c r="F4" s="67"/>
-      <c r="G4" s="67"/>
-      <c r="H4" s="67"/>
+      <c r="B4" s="68"/>
+      <c r="C4" s="68"/>
+      <c r="D4" s="68"/>
+      <c r="E4" s="68"/>
+      <c r="F4" s="68"/>
+      <c r="G4" s="68"/>
+      <c r="H4" s="68"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
@@ -1676,13 +1674,13 @@
       <c r="A5" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="67"/>
-      <c r="C5" s="67"/>
-      <c r="D5" s="67"/>
-      <c r="E5" s="67"/>
-      <c r="F5" s="67"/>
-      <c r="G5" s="67"/>
-      <c r="H5" s="67"/>
+      <c r="B5" s="68"/>
+      <c r="C5" s="68"/>
+      <c r="D5" s="68"/>
+      <c r="E5" s="68"/>
+      <c r="F5" s="68"/>
+      <c r="G5" s="68"/>
+      <c r="H5" s="68"/>
       <c r="I5" s="1"/>
       <c r="J5" s="40"/>
     </row>
@@ -1690,13 +1688,13 @@
       <c r="A6" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="67"/>
-      <c r="C6" s="67"/>
-      <c r="D6" s="67"/>
-      <c r="E6" s="67"/>
-      <c r="F6" s="67"/>
-      <c r="G6" s="67"/>
-      <c r="H6" s="67"/>
+      <c r="B6" s="68"/>
+      <c r="C6" s="68"/>
+      <c r="D6" s="68"/>
+      <c r="E6" s="68"/>
+      <c r="F6" s="68"/>
+      <c r="G6" s="68"/>
+      <c r="H6" s="68"/>
       <c r="I6" s="1"/>
       <c r="J6" s="40"/>
     </row>
@@ -1704,13 +1702,13 @@
       <c r="A7" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="67"/>
-      <c r="C7" s="67"/>
-      <c r="D7" s="67"/>
-      <c r="E7" s="67"/>
-      <c r="F7" s="67"/>
-      <c r="G7" s="67"/>
-      <c r="H7" s="67"/>
+      <c r="B7" s="68"/>
+      <c r="C7" s="68"/>
+      <c r="D7" s="68"/>
+      <c r="E7" s="68"/>
+      <c r="F7" s="68"/>
+      <c r="G7" s="68"/>
+      <c r="H7" s="68"/>
       <c r="I7" s="1"/>
       <c r="J7" s="40"/>
     </row>
@@ -1718,13 +1716,13 @@
       <c r="A8" s="75" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="67"/>
-      <c r="C8" s="67"/>
-      <c r="D8" s="67"/>
-      <c r="E8" s="67"/>
-      <c r="F8" s="67"/>
-      <c r="G8" s="67"/>
-      <c r="H8" s="67"/>
+      <c r="B8" s="68"/>
+      <c r="C8" s="68"/>
+      <c r="D8" s="68"/>
+      <c r="E8" s="68"/>
+      <c r="F8" s="68"/>
+      <c r="G8" s="68"/>
+      <c r="H8" s="68"/>
       <c r="I8" s="40"/>
       <c r="J8" s="40"/>
     </row>
@@ -1744,43 +1742,43 @@
       <c r="A10" s="74" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="69"/>
-      <c r="C10" s="69"/>
-      <c r="D10" s="69"/>
-      <c r="E10" s="69"/>
+      <c r="B10" s="70"/>
+      <c r="C10" s="70"/>
+      <c r="D10" s="70"/>
+      <c r="E10" s="70"/>
       <c r="F10" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="G10" s="68">
+      <c r="G10" s="66"/>
+      <c r="H10" s="66">
         <v>43801</v>
       </c>
-      <c r="H10" s="69"/>
     </row>
     <row r="11" spans="1:17" s="16" customFormat="1" ht="12.75" customHeight="1">
       <c r="A11" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="69"/>
-      <c r="C11" s="69"/>
-      <c r="D11" s="69"/>
-      <c r="E11" s="69"/>
+      <c r="B11" s="70"/>
+      <c r="C11" s="70"/>
+      <c r="D11" s="70"/>
+      <c r="E11" s="70"/>
       <c r="F11" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="G11" s="68">
+      <c r="G11" s="66"/>
+      <c r="H11" s="66">
         <v>43801</v>
       </c>
-      <c r="H11" s="69"/>
     </row>
     <row r="12" spans="1:17" s="16" customFormat="1" ht="12.75" customHeight="1">
       <c r="A12" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="70">
+      <c r="F12" s="69">
         <v>12148</v>
       </c>
-      <c r="G12" s="69"/>
-      <c r="H12" s="69"/>
+      <c r="G12" s="70"/>
+      <c r="H12" s="70"/>
     </row>
     <row r="13" spans="1:17" s="16" customFormat="1" ht="12.75" customHeight="1">
       <c r="A13" s="16" t="s">
@@ -1796,13 +1794,13 @@
       <c r="A15" s="71" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="69"/>
-      <c r="C15" s="69"/>
-      <c r="D15" s="69"/>
-      <c r="E15" s="69"/>
-      <c r="F15" s="69"/>
-      <c r="G15" s="69"/>
-      <c r="H15" s="69"/>
+      <c r="B15" s="70"/>
+      <c r="C15" s="70"/>
+      <c r="D15" s="70"/>
+      <c r="E15" s="70"/>
+      <c r="F15" s="70"/>
+      <c r="G15" s="70"/>
+      <c r="H15" s="70"/>
       <c r="I15" s="36"/>
       <c r="J15" s="20"/>
     </row>
@@ -2251,9 +2249,9 @@
       <c r="G55" s="16"/>
     </row>
     <row r="56" spans="1:8">
-      <c r="F56" s="66"/>
-      <c r="G56" s="67"/>
-      <c r="H56" s="67"/>
+      <c r="F56" s="67"/>
+      <c r="G56" s="68"/>
+      <c r="H56" s="68"/>
     </row>
     <row r="57" spans="1:8">
       <c r="A57" s="16"/>
@@ -2268,9 +2266,8 @@
       <c r="H60" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="11">
     <mergeCell ref="F56:H56"/>
-    <mergeCell ref="G11:H11"/>
     <mergeCell ref="F12:H12"/>
     <mergeCell ref="A15:H15"/>
     <mergeCell ref="A1:H3"/>
@@ -2278,7 +2275,6 @@
     <mergeCell ref="A10:E10"/>
     <mergeCell ref="A11:E11"/>
     <mergeCell ref="A8:H8"/>
-    <mergeCell ref="G10:H10"/>
     <mergeCell ref="A4:H4"/>
     <mergeCell ref="A6:H6"/>
     <mergeCell ref="A7:H7"/>

</xml_diff>